<commit_message>
Phần 2 Admin Pages, 2. chức năng thêm sản phẩm, 3. chức năng xóa sản phẩm
</commit_message>
<xml_diff>
--- a/template_task.xlsx
+++ b/template_task.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -160,7 +160,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,6 +197,18 @@
         <bgColor rgb="FFAEABAB"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor rgb="FFAEABAB"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -365,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -461,6 +473,22 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -705,7 +733,7 @@
   <dimension ref="A1:J986"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -776,18 +804,18 @@
       <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="13"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="40"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
@@ -849,10 +877,18 @@
       <c r="A8" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
+      <c r="B8" s="8">
+        <v>45826</v>
+      </c>
+      <c r="C8" s="11">
+        <v>45826</v>
+      </c>
+      <c r="D8" s="9">
+        <v>1</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>24</v>
+      </c>
       <c r="F8" s="11"/>
       <c r="G8" s="8"/>
       <c r="H8" s="12"/>
@@ -860,27 +896,35 @@
       <c r="J8" s="13"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="13"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="40"/>
     </row>
     <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10"/>
+      <c r="B10" s="11">
+        <v>45826</v>
+      </c>
+      <c r="C10" s="11">
+        <v>45826</v>
+      </c>
+      <c r="D10" s="9">
+        <v>1</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>24</v>
+      </c>
       <c r="F10" s="11"/>
       <c r="G10" s="8"/>
       <c r="H10" s="12"/>
@@ -891,10 +935,18 @@
       <c r="A11" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="10"/>
+      <c r="B11" s="11">
+        <v>45826</v>
+      </c>
+      <c r="C11" s="11">
+        <v>45826</v>
+      </c>
+      <c r="D11" s="9">
+        <v>1</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>24</v>
+      </c>
       <c r="F11" s="11"/>
       <c r="G11" s="8"/>
       <c r="H11" s="12"/>
@@ -905,10 +957,18 @@
       <c r="A12" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="17"/>
+      <c r="B12" s="11">
+        <v>45826</v>
+      </c>
+      <c r="C12" s="11">
+        <v>45826</v>
+      </c>
+      <c r="D12" s="9">
+        <v>1</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>24</v>
+      </c>
       <c r="F12" s="11"/>
       <c r="G12" s="8"/>
       <c r="H12" s="12"/>

</xml_diff>

<commit_message>
Phần 2 Admin Pages, 4. Phần cập nhật sản phẩm, 5. Validation
</commit_message>
<xml_diff>
--- a/template_task.xlsx
+++ b/template_task.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -210,7 +210,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -353,17 +353,6 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -377,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -443,17 +432,11 @@
     <xf numFmtId="164" fontId="2" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="3" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -461,9 +444,6 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -493,7 +473,29 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -732,8 +734,8 @@
   </sheetPr>
   <dimension ref="A1:J986"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -804,18 +806,18 @@
       <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="40"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="37"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
@@ -896,18 +898,18 @@
       <c r="J8" s="13"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="40"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="37"/>
     </row>
     <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
@@ -979,57 +981,73 @@
       <c r="A13" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="24"/>
+      <c r="B13" s="22">
+        <v>45830</v>
+      </c>
+      <c r="C13" s="22">
+        <v>45830</v>
+      </c>
+      <c r="D13" s="9">
+        <v>1</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>24</v>
+      </c>
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="27"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="25"/>
     </row>
     <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="33"/>
+      <c r="B14" s="22">
+        <v>45830</v>
+      </c>
+      <c r="C14" s="22">
+        <v>45830</v>
+      </c>
+      <c r="D14" s="9">
+        <v>1</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="30"/>
     </row>
     <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
     </row>
     <row r="16" spans="1:10" ht="24" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
     </row>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2003,12 +2021,12 @@
     <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="D2:D14">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H16">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Phần 2 Pages Admin. Đã hoàn thành phần tìm kiếm và lọc giá sản phẩm
</commit_message>
<xml_diff>
--- a/template_task.xlsx
+++ b/template_task.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -74,9 +74,6 @@
     <t>2.3 Tạo ô tìm kiếm</t>
   </si>
   <si>
-    <t>2.4 Tạo giỏ hàng bằng Modal</t>
-  </si>
-  <si>
     <t>3. Tạo trang admin hiển thị dữ liệu</t>
   </si>
   <si>
@@ -105,6 +102,12 @@
   </si>
   <si>
     <t>Kỳ Hảo</t>
+  </si>
+  <si>
+    <t>Vũ Luân</t>
+  </si>
+  <si>
+    <t>2.4 Tạo giỏ hàng</t>
   </si>
 </sst>
 </file>
@@ -210,7 +213,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -362,11 +365,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -392,9 +425,6 @@
     <xf numFmtId="164" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -405,17 +435,11 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -459,21 +483,84 @@
     <xf numFmtId="164" fontId="2" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -734,8 +821,8 @@
   </sheetPr>
   <dimension ref="A1:J986"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -787,267 +874,315 @@
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="34">
         <v>45826</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="34">
         <v>45826</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="39">
         <v>1</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="11"/>
+      <c r="E2" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="10"/>
       <c r="G2" s="8"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="13"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="33"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="11"/>
+      <c r="B4" s="34">
+        <v>45826</v>
+      </c>
+      <c r="C4" s="34">
+        <v>45826</v>
+      </c>
+      <c r="D4" s="39">
+        <v>1</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="10"/>
       <c r="G4" s="8"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="13"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="12"/>
     </row>
     <row r="5" spans="1:10" ht="14.25" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="15"/>
+      <c r="B5" s="34">
+        <v>45831</v>
+      </c>
+      <c r="C5" s="34">
+        <v>45831</v>
+      </c>
+      <c r="D5" s="39">
+        <v>1</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="13"/>
       <c r="G5" s="8"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="13"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="15"/>
+      <c r="B6" s="34">
+        <v>45831</v>
+      </c>
+      <c r="C6" s="34">
+        <v>45831</v>
+      </c>
+      <c r="D6" s="39">
+        <v>1</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="13"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="13"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:10" ht="19.2" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="15"/>
+      <c r="A7" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="34">
+        <v>45831</v>
+      </c>
+      <c r="C7" s="34">
+        <v>45831</v>
+      </c>
+      <c r="D7" s="39">
+        <v>1</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="13"/>
       <c r="G7" s="8"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="16"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="14"/>
     </row>
     <row r="8" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="8">
+      <c r="A8" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="34">
         <v>45826</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="34">
         <v>45826</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="39">
         <v>1</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="11"/>
+      <c r="E8" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="10"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="13"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="12"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="37"/>
+      <c r="A9" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="33"/>
     </row>
     <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="11">
+      <c r="A10" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="34">
         <v>45826</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="34">
         <v>45826</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="39">
         <v>1</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="11"/>
+      <c r="E10" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="10"/>
       <c r="G10" s="8"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="13"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="12"/>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="11">
+      <c r="A11" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="34">
         <v>45826</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="34">
         <v>45826</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="39">
         <v>1</v>
       </c>
-      <c r="E11" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="11"/>
+      <c r="E11" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="10"/>
       <c r="G11" s="8"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="13"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="12"/>
     </row>
     <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="11">
+      <c r="A12" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="34">
         <v>45826</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="34">
         <v>45826</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="39">
         <v>1</v>
       </c>
-      <c r="E12" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="11"/>
+      <c r="E12" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="10"/>
       <c r="G12" s="8"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="13"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="12"/>
     </row>
     <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="22">
+      <c r="A13" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="38">
         <v>45830</v>
       </c>
-      <c r="C13" s="22">
+      <c r="C13" s="38">
         <v>45830</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="39">
         <v>1</v>
       </c>
-      <c r="E13" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="25"/>
+      <c r="E13" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="22"/>
     </row>
     <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="22">
+      <c r="A14" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="38">
         <v>45830</v>
       </c>
-      <c r="C14" s="22">
+      <c r="C14" s="38">
         <v>45830</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="39">
         <v>1</v>
       </c>
-      <c r="E14" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="30"/>
+      <c r="E14" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="27"/>
     </row>
     <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
+      <c r="A15" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="38">
+        <v>45830</v>
+      </c>
+      <c r="C15" s="38">
+        <v>45830</v>
+      </c>
+      <c r="D15" s="39">
+        <v>1</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
     </row>
     <row r="16" spans="1:10" ht="24" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="42">
+        <v>45830</v>
+      </c>
+      <c r="C16" s="42">
+        <v>45830</v>
+      </c>
+      <c r="D16" s="43">
+        <v>1</v>
+      </c>
+      <c r="E16" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
     </row>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2020,13 +2155,18 @@
     <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="D2:D14">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="D2:D3 D8:D16">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H16">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D7">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>